<commit_message>
Updated report, added analysis files
</commit_message>
<xml_diff>
--- a/AkronAshevilleTables.xlsx
+++ b/AkronAshevilleTables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/var/mobile/Containers/Data/Application/F3B23897-18E5-4298-8D5E-31F86D26BE47/Library/Application Support/Drafts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{46C2D7EA-09D4-D945-B8D5-11CF521DB2A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{CC96711E-D2ED-D64D-A2AC-02266D1F462D}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{46C2D7EA-09D4-D945-B8D5-11CF521DB2A8}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{BFEE9026-DC34-8E40-B2CC-7305D0A5B6A3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DataField" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="34">
   <si>
     <t>Field Name</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>Descriptive Statistics For Asheville Winter</t>
+  </si>
+  <si>
+    <t>Descriptive Statistics for Akron Summer</t>
+  </si>
+  <si>
+    <t>Descriptive Statistics For Asheville Summer</t>
   </si>
 </sst>
 </file>
@@ -222,6 +228,201 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>165067</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>143820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>174067</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152820</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F235B866-6780-124B-B2AA-BF5747AF2A91}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6786000" y="1858320"/>
+            <a:ext cx="9000" cy="9000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="2" name="Ink 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F235B866-6780-124B-B2AA-BF5747AF2A91}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6770520" y="1842840"/>
+              <a:ext cx="39240" cy="39240"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>219787</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>143820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>237067</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>156780</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EBC6255-37C1-A44D-B7FB-DA81F1D82200}"/>
+                </a:ext>
+                <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+                  <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F235B866-6780-124B-B2AA-BF5747AF2A91}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6840720" y="1858320"/>
+            <a:ext cx="17280" cy="12960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="3" name="Ink 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EBC6255-37C1-A44D-B7FB-DA81F1D82200}"/>
+                </a:ext>
+                <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+                  <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F235B866-6780-124B-B2AA-BF5747AF2A91}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6825600" y="1842840"/>
+              <a:ext cx="47880" cy="43560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-12-02T18:52:41.946"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.08571" units="cm"/>
+      <inkml:brushProperty name="height" value="0.08571" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">0 24 7569,'1'-7'0,"2"2"0,1 0 0,5 4 0,-2-5 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="F" type="integer" max="32767" units="dev"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="F" name="resolution" value="0" units="1/dev"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2018-12-02T18:52:42.920"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.08571" units="cm"/>
+      <inkml:brushProperty name="height" value="0.08571" units="cm"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">36 36 7569,'5'-7'-11,"-3"2"1,3 5-262,-5 0 56,0-5 1,-1 3 21,-3-2 1,1 3-352,-5 1 545,0 0 0,-3-5 0,-1-2 0</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -585,10 +786,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{775CD1DE-1489-8B49-8D2C-72D5E33095EB}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{65553AA6-24FB-5975-A085-6D0509949AFB}">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{65553AA6-24FB-5975-A085-6D0509949AFB}">
+      <selection activeCell="G10" sqref="G10:H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -596,9 +797,11 @@
     <col min="1" max="1" width="29.99609375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="28.11328125" customWidth="1"/>
     <col min="5" max="5" width="9.4140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.88671875" customWidth="1"/>
+    <col min="8" max="8" width="11.56640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>11</v>
       </c>
@@ -607,8 +810,12 @@
         <v>30</v>
       </c>
       <c r="E1" s="5"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>12</v>
@@ -617,8 +824,12 @@
       <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -631,8 +842,14 @@
       <c r="E3" s="1">
         <v>361</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" s="1">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>13</v>
       </c>
@@ -645,8 +862,14 @@
       <c r="E4" s="1">
         <v>29.700831000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="1">
+        <v>71.774456999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>19</v>
       </c>
@@ -659,8 +882,14 @@
       <c r="E5" s="1">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>14</v>
       </c>
@@ -673,8 +902,14 @@
       <c r="E6" s="1">
         <v>13.163679999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="1">
+        <v>5.222118</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>15</v>
       </c>
@@ -687,8 +922,14 @@
       <c r="E7" s="1">
         <v>-6</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -701,8 +942,14 @@
       <c r="E8" s="1">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -711,8 +958,12 @@
         <v>31</v>
       </c>
       <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G10" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
@@ -721,8 +972,12 @@
       <c r="E11" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
@@ -735,8 +990,14 @@
       <c r="E12" s="3">
         <v>361</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H12" s="3">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -749,8 +1010,14 @@
       <c r="E13" s="1">
         <v>39.936287999999998</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="1">
+        <v>72.633151999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
@@ -763,8 +1030,14 @@
       <c r="E14" s="1">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H14" s="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -777,8 +1050,14 @@
       <c r="E15" s="1">
         <v>10.420004</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="1">
+        <v>3.276319</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
@@ -791,8 +1070,14 @@
       <c r="E16" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -805,15 +1090,24 @@
       <c r="E17" s="1">
         <v>64</v>
       </c>
+      <c r="G17" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="1">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G10:H10"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A10:B10"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -821,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E03E75B-F3AF-E94E-8610-E17BC0ED2700}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{EF3162B9-7748-5A64-A985-1EB489C58AA6}">
+    <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0" xr3:uid="{EF3162B9-7748-5A64-A985-1EB489C58AA6}">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>